<commit_message>
WVC - Work Modes - 2888380373 업데이트
</commit_message>
<xml_diff>
--- a/Data/WVC - Work Modes - 2888380373/1.5/2888380373.xlsx
+++ b/Data/WVC - Work Modes - 2888380373/1.5/2888380373.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.8.6\WVC - Work Modes - 2888380373\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\WVC - Work Modes - 2888380373\1.5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA8A13A-9CA8-44BA-A669-48A038EE5754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46D1E64-A39C-4869-9B3F-ACBFD03989A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main_240602" sheetId="1" r:id="rId1"/>
@@ -32,8 +32,200 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>bjmi0</author>
+  </authors>
+  <commentList>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-08-04에 삭제됨. 삭제 이전 번역문: 'WVC'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-08-04 이전의 원문: 'Mechanoids, regardless of type, will generate research points relative to their bandwidth cost. The speed and efficiency of research directly depends on the number of mechanoids involved in it.
+If there is an enemy on the map or in case of damage, the mechanoids will head to a safe zone.
+&lt;color=#f5ffa2&gt;Type:&lt;/color&gt; Safe
+&lt;color=#f5ffa2&gt;Enemy searching:&lt;/color&gt; No
+&lt;color=#f5ffa2&gt;Shutdown:&lt;/color&gt; If damaged
+&lt;color=#f5ffa2&gt;Smart charging:&lt;/color&gt; Yes'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">2025-08-04 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>이전의</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>원문</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>: 'Mechanoids, regardless of type, will search for useful resources in special "Scavenge" zones.
+If there is an enemy on the map or in case of damage, the mechanoids will head to a safe zone.
+&lt;color=#f5ffa2&gt;Type:&lt;/color&gt; Safe
+&lt;color=#f5ffa2&gt;Enemy searching:&lt;/color&gt; No
+&lt;color=#f5ffa2&gt;Shutdown:&lt;/color&gt; If damaged
+&lt;color=#f5ffa2&gt;Smart charging:&lt;/color&gt; Yes'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-08-04 이전의 원문: 'Mechanoids, regardless of their type, will look for enemies and try to destroy them.
+&lt;color=#f5ffa2&gt;Type:&lt;/color&gt; Combat
+&lt;color=#f5ffa2&gt;Enemy searching:&lt;/color&gt; Yes
+&lt;color=#f5ffa2&gt;Shutdown:&lt;/color&gt; No
+&lt;color=#f5ffa2&gt;Smart charging:&lt;/color&gt; Yes'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-08-04에 삭제됨. 삭제 이전 번역문: '메카나이터가 메카노이드에게 고급 작업 명령을 내릴 수 있습니다.'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E35" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-08-04에 삭제됨. 삭제 이전 번역문: '기계 연구'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E36" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-08-04에 삭제됨. 삭제 이전 번역문: '메카나이터가 메카노이드에게 고급 작업 명령을 내릴 수 있습니다.'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-08-04에 삭제됨. 삭제 이전 번역문: '기계 수집'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E106" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-08-04 이전의 원문: 'Enable shutdown zone searching'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E121" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-08-04에 새로 추가된 노드들 (9개)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="494">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -75,6 +267,9 @@
   </si>
   <si>
     <t>More Mechanoids Work Modes - Behaviors</t>
+  </si>
+  <si>
+    <t>더 많은 메카노이드 작업 모드 - 동작들</t>
   </si>
   <si>
     <t>ConceptDef+WVC_MMWM_BehaviorsGuide.description</t>
@@ -99,6 +294,22 @@
 Smart escort - Mechanoids can be assigned an escort purpose. This way the mechanoids will be able to protect and accompany different pawns. This feature only works for the home map.</t>
   </si>
   <si>
+    <t>이 모드는 알아두어야 할 몇 가지 독특한 동작을 추가합니다.
+-
+지도에서 적을 확인합니다. 적이 접근 가능하고 메카노이드가 작동하는 영역에 없다면 메카노이드는 정상적으로 작동을 계속합니다.
+무엇을 의미하는가:
+"안전한 경우 작업" 모드를 활성화하고 작업 영역을 제한하면, 메카노이드는 적이 메카노이드의 작업 영역에 들어올 때까지 침입을 무시합니다.
+"소탕" 모드를 활성화하고 메카노이드를 작지만 개방된 영역에 고정시킨 경우, 메카노이드는 적을 추적하지 않고 메카노이드의 시야에 있는 적과 싸우려고 할 것입니다. 지나치게 스마트한 적 AI 모드를 깔았다면 메카노이드를 카이팅할 수도 있습니다.
+-
+자동 충전 - 일부 모드에서 메카노이드는 최대 충전량에 가깝도록 유지하려고 합니다. 이는 다음 공식에 따라 계산됩니다 (최대 충전 수준 - 5). 즉, 충전을 100%로 설정하면 메카노이드는 95%까지 충전됩니다. 그러나 기본 충전과 달리, 필요한 경우 메카노이드는 충전을 중단합니다.
+-
+대기 모드 - 일부 작업 모드에서는 아무것도 하지 않을 때 최적화를 위해 메카노이드를 비활성화합니다. 작업 모드에서는 재사용 대기시간이 전투 모드보다 훨씬 길어집니다.
+-
+메카노이드 대기 구역 - 모든 업무를 마치고 잠들려고 하는 메카노이드는 접근 가능한 구역에 있는 경우 가장 가까운 구역으로 이동합니다.
+-
+스마트 호위 - 메카노이드에 호위 대상을 지정할 수 있습니다. 메카노이드가 다른 폰을 보호하고 동행합니다. 이 기능은 정착지에서만 작동합니다.</t>
+  </si>
+  <si>
     <t>ConceptDef+WVC_MMWM_BehaviorsGuide.helpText</t>
   </si>
   <si>
@@ -133,6 +344,9 @@
     <t>safe yourself</t>
   </si>
   <si>
+    <t>자율 방어</t>
+  </si>
+  <si>
     <t>MechWorkModeDef+WVC_DefendYourself.description</t>
   </si>
   <si>
@@ -155,18 +369,20 @@
     <t>hive mind research</t>
   </si>
   <si>
+    <t>대역폭 연구</t>
+  </si>
+  <si>
     <t>MechWorkModeDef+WVC_HiveMindResearching.description</t>
   </si>
   <si>
     <t>WVC_HiveMindResearching.description</t>
   </si>
   <si>
-    <t>Mechanoids, regardless of type, will generate research points relative to their bandwidth cost. The speed and efficiency of research directly depends on the number of mechanoids involved in it.
-If there is an enemy on the map or in case of damage, the mechanoids will head to a safe zone.
+    <t>Mechanoids, regardless of type, will search for useful resources in special "Scavenge" zones. If there is an enemy on the map or in case of damage, the mechanoids will head to a safe zone.
 &lt;color=#f5ffa2&gt;Type:&lt;/color&gt; Safe
-&lt;color=#f5ffa2&gt;Enemy searching:&lt;/color&gt; No
+&lt;color=#f5ffa2&gt;Enemy searching:&lt;/color&gt; Yes
 &lt;color=#f5ffa2&gt;Shutdown:&lt;/color&gt; If damaged
-&lt;color=#f5ffa2&gt;Smart charging:&lt;/color&gt; Yes</t>
+&lt;color=#f5ffa2&gt;Smart charging:&lt;/color&gt; No</t>
   </si>
   <si>
     <t>MechWorkModeDef+WVC_Scavenging.label</t>
@@ -178,40 +394,41 @@
     <t>scavenging</t>
   </si>
   <si>
+    <t>수집</t>
+  </si>
+  <si>
     <t>MechWorkModeDef+WVC_Scavenging.description</t>
   </si>
   <si>
     <t>WVC_Scavenging.description</t>
-  </si>
-  <si>
-    <t>Mechanoids, regardless of type, will search for useful resources in special "Scavenge" zones.
-If there is an enemy on the map or in case of damage, the mechanoids will head to a safe zone.
-&lt;color=#f5ffa2&gt;Type:&lt;/color&gt; Safe
-&lt;color=#f5ffa2&gt;Enemy searching:&lt;/color&gt; No
-&lt;color=#f5ffa2&gt;Shutdown:&lt;/color&gt; If damaged
-&lt;color=#f5ffa2&gt;Smart charging:&lt;/color&gt; Yes</t>
-  </si>
-  <si>
-    <t>MechWorkModeDef+WVC_FindAndDestroy.label</t>
-  </si>
-  <si>
-    <t>WVC_FindAndDestroy.label</t>
-  </si>
-  <si>
-    <t>find and destroy</t>
-  </si>
-  <si>
-    <t>MechWorkModeDef+WVC_FindAndDestroy.description</t>
-  </si>
-  <si>
-    <t>WVC_FindAndDestroy.description</t>
   </si>
   <si>
     <t>Mechanoids, regardless of their type, will look for enemies and try to destroy them.
 &lt;color=#f5ffa2&gt;Type:&lt;/color&gt; Combat
 &lt;color=#f5ffa2&gt;Enemy searching:&lt;/color&gt; Yes
 &lt;color=#f5ffa2&gt;Shutdown:&lt;/color&gt; No
-&lt;color=#f5ffa2&gt;Smart charging:&lt;/color&gt; Yes</t>
+&lt;color=#f5ffa2&gt;Smart charging:&lt;/color&gt; No</t>
+  </si>
+  <si>
+    <t>MechWorkModeDef+WVC_FindAndDestroy.label</t>
+  </si>
+  <si>
+    <t>WVC_FindAndDestroy.label</t>
+  </si>
+  <si>
+    <t>find and destroy</t>
+  </si>
+  <si>
+    <t>소탕</t>
+  </si>
+  <si>
+    <t>MechWorkModeDef+WVC_FindAndDestroy.description</t>
+  </si>
+  <si>
+    <t>WVC_FindAndDestroy.description</t>
+  </si>
+  <si>
+    <t>Enable mechanoid shutdown zones</t>
   </si>
   <si>
     <t>MechWorkModeDef+WVC_WaitEnemy.label</t>
@@ -221,6 +438,9 @@
   </si>
   <si>
     <t>wait enemy</t>
+  </si>
+  <si>
+    <t>전투 대기</t>
   </si>
   <si>
     <t>MechWorkModeDef+WVC_WaitEnemy.description</t>
@@ -245,6 +465,9 @@
     <t>work and wait</t>
   </si>
   <si>
+    <t>작업 및 전투</t>
+  </si>
+  <si>
     <t>MechWorkModeDef+WVC_WorkAndWaitEnemy.description</t>
   </si>
   <si>
@@ -267,6 +490,9 @@
     <t>ambush</t>
   </si>
   <si>
+    <t>매복</t>
+  </si>
+  <si>
     <t>MechWorkModeDef+WVC_Ambush.description</t>
   </si>
   <si>
@@ -289,6 +515,9 @@
     <t>work and recharge</t>
   </si>
   <si>
+    <t>작업 및 충전</t>
+  </si>
+  <si>
     <t>MechWorkModeDef+WVC_WorkAndRecharge.description</t>
   </si>
   <si>
@@ -311,6 +540,9 @@
     <t>work if safe</t>
   </si>
   <si>
+    <t>작업 및 대피</t>
+  </si>
+  <si>
     <t>MechWorkModeDef+WVC_SafeWorkAndRecharge.description</t>
   </si>
   <si>
@@ -333,6 +565,9 @@
     <t>work, recharge and escort</t>
   </si>
   <si>
+    <t>작업, 충전 및 호위</t>
+  </si>
+  <si>
     <t>MechWorkModeDef+WVC_WorkRechargeEscort.description</t>
   </si>
   <si>
@@ -355,6 +590,9 @@
     <t>escort if enemy, work and recharge</t>
   </si>
   <si>
+    <t>작업, 충전 및 적이 있을 경우 호위</t>
+  </si>
+  <si>
     <t>MechWorkModeDef+WVC_EscortIfEnemyWorkAndRecharge.description</t>
   </si>
   <si>
@@ -377,6 +615,9 @@
     <t>escort if drafted or downed</t>
   </si>
   <si>
+    <t>소집되거나 쓰러질 경우 호위</t>
+  </si>
+  <si>
     <t>MechWorkModeDef+WVC_EscortIfDraftedOrDowned.description</t>
   </si>
   <si>
@@ -399,6 +640,9 @@
     <t>escort if enemy</t>
   </si>
   <si>
+    <t>적이 있을 경우 호위</t>
+  </si>
+  <si>
     <t>MechWorkModeDef+WVC_EscortIfEnemyOnMap.description</t>
   </si>
   <si>
@@ -421,6 +665,9 @@
     <t>escort and recharge</t>
   </si>
   <si>
+    <t>충전 및 호위</t>
+  </si>
+  <si>
     <t>MechWorkModeDef+WVC_EscaortAndRecharge.description</t>
   </si>
   <si>
@@ -446,6 +693,9 @@
     <t>Allows the mechanitor to use of advanced work modes for mechanoid groups.</t>
   </si>
   <si>
+    <t>WVC_RechargeAndShutdown.label</t>
+  </si>
+  <si>
     <t>ResearchProjectDef+WVC_WorkModes_HiveMindResearch.label</t>
   </si>
   <si>
@@ -470,6 +720,13 @@
     <t>scavenging mode</t>
   </si>
   <si>
+    <t>Mechanoids, regardless of type, will generate research points. If there is an enemy on the map or in case of damage, the mechanoids will head to a safe zone.
+&lt;color=#f5ffa2&gt;Type:&lt;/color&gt; Safe
+&lt;color=#f5ffa2&gt;Enemy searching:&lt;/color&gt; Yes
+&lt;color=#f5ffa2&gt;Shutdown:&lt;/color&gt; If damaged
+&lt;color=#f5ffa2&gt;Smart charging:&lt;/color&gt; No</t>
+  </si>
+  <si>
     <t>Keyed+WVC_MechanoidShutdownZone</t>
   </si>
   <si>
@@ -482,6 +739,9 @@
     <t>Mechanoid shutdown zone</t>
   </si>
   <si>
+    <t>메카노이드 대기 구역</t>
+  </si>
+  <si>
     <t>Keyed+WVC_MechanoidShutdownZoneDesc</t>
   </si>
   <si>
@@ -491,6 +751,9 @@
     <t>Mechanoids will return here before shutting down.</t>
   </si>
   <si>
+    <t>메카노이드는 이곳으로 돌아와 대기합니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_ShutdownZone_AllowWorkers</t>
   </si>
   <si>
@@ -500,6 +763,9 @@
     <t>Work type</t>
   </si>
   <si>
+    <t>노동 유형</t>
+  </si>
+  <si>
     <t>Keyed+WVC_ShutdownZone_AllowSafe</t>
   </si>
   <si>
@@ -509,6 +775,9 @@
     <t>Safe type</t>
   </si>
   <si>
+    <t>안전 유형</t>
+  </si>
+  <si>
     <t>Keyed+WVC_ShutdownZone_AllowCombatants</t>
   </si>
   <si>
@@ -518,6 +787,9 @@
     <t>Combat type</t>
   </si>
   <si>
+    <t>전투 유형</t>
+  </si>
+  <si>
     <t>Keyed+WVC_ShutdownZone_AllowAmbush</t>
   </si>
   <si>
@@ -527,6 +799,9 @@
     <t>Ambush type</t>
   </si>
   <si>
+    <t>매복 유형</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_allowAllGroups</t>
   </si>
   <si>
@@ -536,6 +811,9 @@
     <t>All groups allowed</t>
   </si>
   <si>
+    <t>모든 유형 허용</t>
+  </si>
+  <si>
     <t>Keyed+WVC_ShutdownZone_BasicDesc</t>
   </si>
   <si>
@@ -545,6 +823,9 @@
     <t>Responsible for whether mechanoids with this type of work will be able to shutdown here.</t>
   </si>
   <si>
+    <t>특정 유형의 메카노이드를 이곳에서 대기하도록 합니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_allowAllGroupsDesc</t>
   </si>
   <si>
@@ -554,6 +835,9 @@
     <t>Responsible for whether all mechanoids, regardless of the group, can use this zone.</t>
   </si>
   <si>
+    <t>모든 유형의 메카노이드를 이곳에서 대기하도록 합니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_On</t>
   </si>
   <si>
@@ -581,6 +865,9 @@
     <t>Mechanoid scavenge zone</t>
   </si>
   <si>
+    <t>메카노이드 수집 구역</t>
+  </si>
+  <si>
     <t>Keyed+WVC_MechanoidScavengeZoneDesc</t>
   </si>
   <si>
@@ -599,6 +886,9 @@
     <t>Cells: {0} | Minimum allowed: {1}</t>
   </si>
   <si>
+    <t>셀: {0} | 최소 허용: {1}</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_AssignToPawnEscortLabel</t>
   </si>
   <si>
@@ -608,6 +898,9 @@
     <t>Assign to escort</t>
   </si>
   <si>
+    <t>호위 배정</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_AssignToPawnEscortLabelReset</t>
   </si>
   <si>
@@ -615,6 +908,9 @@
   </si>
   <si>
     <t>Reset escorted pawn</t>
+  </si>
+  <si>
+    <t>호위 대상 초기화</t>
   </si>
   <si>
     <t>Keyed+WVC_WorkModes_AssignToPawnEscortDesc</t>
@@ -628,6 +924,11 @@
 {0} cannot follow anyone other than an overseer in a caravan or on non-home maps.</t>
   </si>
   <si>
+    <t>{0}(이)가 {1}(을)를 호위함
+메카노이드에게 어떤 정착민을 호위할지 지정할 수 있습니다.
+{0}(은)는 상단이나 정착지 외부의 맵에서 감독관 이외의 다른 사람을 따라갈 수 없습니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_AssignToPawnEscortAssigned</t>
   </si>
   <si>
@@ -637,6 +938,9 @@
     <t>{0} assigned to escort {1}.</t>
   </si>
   <si>
+    <t>{0}(이)가 {1}(을)를 호위합니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_AssignToPawnEscortNoLongerEscort</t>
   </si>
   <si>
@@ -646,6 +950,9 @@
     <t>{0} no longer escort {1}.</t>
   </si>
   <si>
+    <t>{0}(이)가 더 이상 {1}(을)를 호위하지 않습니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_EscortsAssignTargetLabel</t>
   </si>
   <si>
@@ -655,6 +962,9 @@
     <t>Assigned to escorts {0}</t>
   </si>
   <si>
+    <t>{0}(을)를 호위합니다</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_ChangeModDefaultMessage</t>
   </si>
   <si>
@@ -667,12 +977,27 @@
     <t>Keyed+WVC_WorkModes_ModeTechnologyRequirement</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>{0}(이)가 연구되지 않아 사용할 수 없습니다. {1} 유형으로 변경됩니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>WVC_WorkModes_ModeTechnologyRequirement</t>
   </si>
   <si>
     <t>Required technologies:</t>
   </si>
   <si>
+    <t>요구 연구:</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_TechnologyAllowsModes</t>
   </si>
   <si>
@@ -682,6 +1007,9 @@
     <t>Allows use new modes:</t>
   </si>
   <si>
+    <t>새로운 작업 유형 사용 가능:</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_TechnologyAllowsModes_Desc</t>
   </si>
   <si>
@@ -700,6 +1028,9 @@
     <t>Current group</t>
   </si>
   <si>
+    <t>현재 그룹</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_CurrentZoneOwner</t>
   </si>
   <si>
@@ -709,6 +1040,9 @@
     <t>Current owner</t>
   </si>
   <si>
+    <t>현재 소유자</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_ChosenGroupLabel</t>
   </si>
   <si>
@@ -718,6 +1052,9 @@
     <t>Assign group</t>
   </si>
   <si>
+    <t>그룹 지정</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_ChosenGroupDesc</t>
   </si>
   <si>
@@ -727,6 +1064,9 @@
     <t>Allows you to designate a group of mechanoids that will return to this zone.</t>
   </si>
   <si>
+    <t>이 구역으로 돌아올 메카노이드 그룹을 지정할 수 있습니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_GroupIsChosen</t>
   </si>
   <si>
@@ -736,6 +1076,9 @@
     <t>Group {0} assigned to {1}.</t>
   </si>
   <si>
+    <t>그룹 {0}(을)를 {1}에 할당했습니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_ChosenMechanitorLabel</t>
   </si>
   <si>
@@ -745,6 +1088,9 @@
     <t>Assign mechanitor</t>
   </si>
   <si>
+    <t>메카나이터 지정</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_ChosenMechanitorDesc</t>
   </si>
   <si>
@@ -754,6 +1100,9 @@
     <t>Allows you to assign a zone owner.</t>
   </si>
   <si>
+    <t>구역 소유자를 지정할 수 있습니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_MechanitorIsChosen</t>
   </si>
   <si>
@@ -763,6 +1112,9 @@
     <t>{0} assigned as owner of {1}.</t>
   </si>
   <si>
+    <t>{0}(이)가 {1}의 소유자로 지정되었습니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_ResetOwnerLabel</t>
   </si>
   <si>
@@ -772,6 +1124,9 @@
     <t>Reset owner</t>
   </si>
   <si>
+    <t>소유자 초기화</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_ResetOwnerDesc</t>
   </si>
   <si>
@@ -781,6 +1136,9 @@
     <t>Allows you to reset a zone owner.</t>
   </si>
   <si>
+    <t>구역 소유자를 초기화할 수 있습니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_ResetOwnerMessage</t>
   </si>
   <si>
@@ -790,6 +1148,9 @@
     <t>{0} settings are reset to default.</t>
   </si>
   <si>
+    <t>{0} 설정을 기본값으로 초기화합니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_RestrictZoneByGroupLabel</t>
   </si>
   <si>
@@ -799,6 +1160,9 @@
     <t>Use only group zones</t>
   </si>
   <si>
+    <t>그룹 구역만 사용</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_RestrictZoneByGroupDesc</t>
   </si>
   <si>
@@ -808,6 +1172,9 @@
     <t>Allows you to limit the mechanoid's choice of zones to those specifically assigned to its group.</t>
   </si>
   <si>
+    <t>메카노이드가 그룹에 할당된 구역 내부에서만 작업하도록 제한할 수 있습니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_RestrictZoneByGroupInspect</t>
   </si>
   <si>
@@ -826,6 +1193,9 @@
     <t>In shutdown mode x{0}%</t>
   </si>
   <si>
+    <t>대기 모드에서 x{0}%</t>
+  </si>
+  <si>
     <t>Keyed+WVC_MMWM_Settings</t>
   </si>
   <si>
@@ -835,6 +1205,9 @@
     <t>Work Modes</t>
   </si>
   <si>
+    <t>작업 유형</t>
+  </si>
+  <si>
     <t>Keyed+WVC_Label_MainModeLabelSetting</t>
   </si>
   <si>
@@ -844,6 +1217,9 @@
     <t>Main</t>
   </si>
   <si>
+    <t>기본</t>
+  </si>
+  <si>
     <t>Keyed+WVC_Label_BonusModeLabelSetting</t>
   </si>
   <si>
@@ -853,6 +1229,9 @@
     <t>Bonus</t>
   </si>
   <si>
+    <t>추가</t>
+  </si>
+  <si>
     <t>Keyed+WVC_Label_WorkModeMechanicsLabelSetting</t>
   </si>
   <si>
@@ -862,6 +1241,9 @@
     <t>Mechanics</t>
   </si>
   <si>
+    <t>상세</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_ResetButton</t>
   </si>
   <si>
@@ -871,6 +1253,9 @@
     <t>Reset</t>
   </si>
   <si>
+    <t>초기화</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_ResetButtonWarning</t>
   </si>
   <si>
@@ -880,6 +1265,9 @@
     <t>The settings will be changed, are you sure?</t>
   </si>
   <si>
+    <t>설정이 변경됩니다. 실행하시겠습니까?</t>
+  </si>
+  <si>
     <t>Keyed+WVC_WorkModes_ResetButton_SettingsChanged</t>
   </si>
   <si>
@@ -889,6 +1277,9 @@
     <t>The settings have been changed.</t>
   </si>
   <si>
+    <t>설정이 변경되었습니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_Label_FindAndDestroy</t>
   </si>
   <si>
@@ -1033,6 +1424,9 @@
     <t>Scavenge zone min required cells: {0}</t>
   </si>
   <si>
+    <t>수집 구역 최소 요구 범위: {0}</t>
+  </si>
+  <si>
     <t>Keyed+WVC_ToolTip_BonusSetting</t>
   </si>
   <si>
@@ -1042,6 +1436,9 @@
     <t>Bonus mode. It is disabled by default. Enabling is compatible with saves.</t>
   </si>
   <si>
+    <t>추가 모드. 기본적으로 비활성화되어 있습니다. 활성화하면 기존 저장과 호환됩니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_Label_enableShutdownForAllMechanoids</t>
   </si>
   <si>
@@ -1051,6 +1448,9 @@
     <t>Idle optimization for vanilla modes</t>
   </si>
   <si>
+    <t>바닐라 모드를 위한 메카노이드 대기 연산 최적화</t>
+  </si>
+  <si>
     <t>Keyed+WVC_ToolTip_enableShutdownForAllMechanoids</t>
   </si>
   <si>
@@ -1060,6 +1460,9 @@
     <t>If enabled, idle optimization will also affect vanilla modes.</t>
   </si>
   <si>
+    <t>활성화하면 대기 연산 최적화가 바닐라 모드에도 영향을 미칩니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_Label_enableSmartChargingForAllMechanoids</t>
   </si>
   <si>
@@ -1069,6 +1472,9 @@
     <t>Smart charging for vanilla modes</t>
   </si>
   <si>
+    <t>바닐라 모드를 위한 스마트 충전</t>
+  </si>
+  <si>
     <t>Keyed+WVC_ToolTip_enableSmartChargingForAllMechanoids</t>
   </si>
   <si>
@@ -1078,6 +1484,9 @@
     <t>If enabled, then the mechanoids will go to charge when they are not busy with anything, and not only when the charge runs out.</t>
   </si>
   <si>
+    <t>이 기능을 활성화하면 메카노이드는 충전이 다 떨어졌을 때뿐만 아니라 아무것도 하지 않을 때에도 충전을 시작합니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_ToolTip_VanillaModeOptimizationWarning</t>
   </si>
   <si>
@@ -1087,13 +1496,16 @@
     <t>Does not affect combat mechanoids, as their idle has been replaced with a simulated patrol.</t>
   </si>
   <si>
+    <t>전투 메카노이드의 유휴 상태가 시뮬레이션 순찰로 대체되었으므로 영향을 미치지 않습니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_Label_enableShutdownSearching</t>
   </si>
   <si>
     <t>WVC_Label_enableShutdownSearching</t>
   </si>
   <si>
-    <t>Enable shutdown zone searching</t>
+    <t>MechWorkModeDef+WVC_RechargeAndShutdown.label</t>
   </si>
   <si>
     <t>Keyed+WVC_ToolTip_enableShutdownSearching</t>
@@ -1105,6 +1517,9 @@
     <t>If enabled, mechanoids will search for a mechanoid shutdown zone before shutdown.</t>
   </si>
   <si>
+    <t>활성화하면 메카노이드가 대기하기 전에 메카노이드 대기 영역을 검색합니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_Label_enableEnemySearching</t>
   </si>
   <si>
@@ -1114,6 +1529,9 @@
     <t>Enable enemy searching</t>
   </si>
   <si>
+    <t>적 탐색 활성화</t>
+  </si>
+  <si>
     <t>Keyed+WVC_ToolTip_enableEnemySearching</t>
   </si>
   <si>
@@ -1123,6 +1541,9 @@
     <t>If enabled, in safe modes, mechanoids will check the map for enemies.</t>
   </si>
   <si>
+    <t>활성화하면 안전 모드에서 메카노이드가 맵에서 적을 확인합니다.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_ToolTip_enableSearchingWarning</t>
   </si>
   <si>
@@ -1132,6 +1553,9 @@
     <t>If you don't understand what this option does, leave it enabled.</t>
   </si>
   <si>
+    <t>이 옵션이 어떤 기능을 하는지 잘 모르겠다면 사용하도록 설정해 두세요.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_Label_enableSmartEscort</t>
   </si>
   <si>
@@ -1139,6 +1563,9 @@
   </si>
   <si>
     <t>Smart escort</t>
+  </si>
+  <si>
+    <t>스마트 호위</t>
   </si>
   <si>
     <t>Keyed+WVC_ToolTip_enableSmartEscort</t>
@@ -1151,6 +1578,10 @@
 Restart required!</t>
   </si>
   <si>
+    <t>활성화하면 메카노이드의 호위 대상을 선택할 수 있습니다.
+재시작이 필요합니다!</t>
+  </si>
+  <si>
     <t>Keyed+WVC_Label_shutdownModeZonesOrSpots</t>
   </si>
   <si>
@@ -1158,6 +1589,9 @@
   </si>
   <si>
     <t>Shutdown mode: Zones or Spots</t>
+  </si>
+  <si>
+    <t>대기 모드: 구역 또는 장소</t>
   </si>
   <si>
     <t>Keyed+WVC_ToolTip_shutdownModeZonesOrSpots</t>
@@ -1171,6 +1605,11 @@
 Restart required!</t>
   </si>
   <si>
+    <t>활성화하면 영역이 사용됩니다. 또는 장소를 사용할 수도 있습니다. 활성화하는 것이 좋습니다.
+이 옵션은 고급 사용자를 위한 옵션입니다. 장소가 무엇인지 모르는 경우에는 활성화된 상태로 두세요.
+재시작이 필요합니다!</t>
+  </si>
+  <si>
     <t>Keyed+WVC_Label_useCustomShutdownBehavior</t>
   </si>
   <si>
@@ -1180,6 +1619,9 @@
     <t>Use custom shutdown behavior</t>
   </si>
   <si>
+    <t>사용자 지정 대기 동작 사용</t>
+  </si>
+  <si>
     <t>Keyed+WVC_ToolTip_useCustomShutdownBehavior</t>
   </si>
   <si>
@@ -1189,6 +1631,9 @@
     <t>Vanilla shutdown is too stupid, but reliable. If you encounter bugs related to mechanoid shutdown, disable this option.</t>
   </si>
   <si>
+    <t>바닐라 대기 상태는 너무 어리석지만 안정적입니다. 메카노이드 종료와 관련된 버그가 발생하면 이 옵션을 비활성화하세요.</t>
+  </si>
+  <si>
     <t>Keyed+WVC_Label_enableDormantMode</t>
   </si>
   <si>
@@ -1196,6 +1641,9 @@
   </si>
   <si>
     <t>Dormant mode</t>
+  </si>
+  <si>
+    <t>휴면 모드</t>
   </si>
   <si>
     <t>Keyed+WVC_ToolTip_enableDormantMode</t>
@@ -1209,382 +1657,213 @@
 Restart required!</t>
   </si>
   <si>
-    <t>Keyed+WVC_Label_mechBandwithCostInDormantMode</t>
-  </si>
-  <si>
-    <t>WVC_Label_mechBandwithCostInDormantMode</t>
-  </si>
-  <si>
-    <t>Dormant mode bandwidth cost factor x{0}%</t>
-  </si>
-  <si>
-    <t>메카노이드 휴면 시 대역폭 x{0}%</t>
-  </si>
-  <si>
     <t>이 옵션을 활성화하면 메카노이드가 종료 모드에 있을 때 대역폭을 소비하지 않습니다.
 성능에 문제가 있는 경우 비활성화하는 것이 좋습니다.
 재시작이 필요합니다!</t>
   </si>
   <si>
-    <t>휴면 모드</t>
-  </si>
-  <si>
-    <t>바닐라 대기 상태는 너무 어리석지만 안정적입니다. 메카노이드 종료와 관련된 버그가 발생하면 이 옵션을 비활성화하세요.</t>
-  </si>
-  <si>
-    <t>사용자 지정 대기 동작 사용</t>
-  </si>
-  <si>
-    <t>활성화하면 영역이 사용됩니다. 또는 장소를 사용할 수도 있습니다. 활성화하는 것이 좋습니다.
-이 옵션은 고급 사용자를 위한 옵션입니다. 장소가 무엇인지 모르는 경우에는 활성화된 상태로 두세요.
-재시작이 필요합니다!</t>
-  </si>
-  <si>
-    <t>대기 모드: 구역 또는 장소</t>
-  </si>
-  <si>
-    <t>활성화하면 메카노이드의 호위 대상을 선택할 수 있습니다.
-재시작이 필요합니다!</t>
-  </si>
-  <si>
-    <t>스마트 호위</t>
-  </si>
-  <si>
-    <t>이 옵션이 어떤 기능을 하는지 잘 모르겠다면 사용하도록 설정해 두세요.</t>
-  </si>
-  <si>
-    <t>활성화하면 안전 모드에서 메카노이드가 맵에서 적을 확인합니다.</t>
-  </si>
-  <si>
-    <t>적 탐색 활성화</t>
-  </si>
-  <si>
-    <t>활성화하면 메카노이드가 대기하기 전에 메카노이드 대기 영역을 검색합니다.</t>
-  </si>
-  <si>
-    <t>대기 구역 검색 활성화</t>
-  </si>
-  <si>
-    <t>전투 메카노이드의 유휴 상태가 시뮬레이션 순찰로 대체되었으므로 영향을 미치지 않습니다.</t>
-  </si>
-  <si>
-    <t>이 기능을 활성화하면 메카노이드는 충전이 다 떨어졌을 때뿐만 아니라 아무것도 하지 않을 때에도 충전을 시작합니다.</t>
-  </si>
-  <si>
-    <t>바닐라 모드를 위한 스마트 충전</t>
-  </si>
-  <si>
-    <t>활성화하면 대기 연산 최적화가 바닐라 모드에도 영향을 미칩니다.</t>
-  </si>
-  <si>
-    <t>바닐라 모드를 위한 메카노이드 대기 연산 최적화</t>
-  </si>
-  <si>
-    <t>추가 모드. 기본적으로 비활성화되어 있습니다. 활성화하면 기존 저장과 호환됩니다.</t>
-  </si>
-  <si>
-    <t>수집 구역 최소 요구 범위: {0}</t>
-  </si>
-  <si>
-    <t>수집</t>
-  </si>
-  <si>
-    <t>대역폭 연구</t>
-  </si>
-  <si>
-    <t>소집되거나 쓰러질 경우 호위</t>
-  </si>
-  <si>
-    <t>작업, 충전 및 적이 있을 경우 호위</t>
-  </si>
-  <si>
-    <t>비활성화하기 전에 모든 메카노이드 모드를 바닐라로 전환하세요. 설정을 적용하려면 재시작해야 합니다.</t>
-  </si>
-  <si>
-    <t>적이 있을 경우 호위</t>
-  </si>
-  <si>
-    <t>작업, 충전 및 호위</t>
-  </si>
-  <si>
-    <t>충전 및 호위</t>
-  </si>
-  <si>
-    <t>작업 및 대피</t>
-  </si>
-  <si>
-    <t>작업 및 충전</t>
-  </si>
-  <si>
-    <t>매복</t>
-  </si>
-  <si>
-    <t>자율 방어</t>
-  </si>
-  <si>
-    <t>작업 및 전투</t>
-  </si>
-  <si>
-    <t>전투 대기</t>
-  </si>
-  <si>
-    <t>소탕</t>
-  </si>
-  <si>
-    <t>설정이 변경되었습니다.</t>
-  </si>
-  <si>
-    <t>설정이 변경됩니다. 실행하시겠습니까?</t>
-  </si>
-  <si>
-    <t>초기화</t>
-  </si>
-  <si>
-    <t>상세</t>
-  </si>
-  <si>
-    <t>추가</t>
-  </si>
-  <si>
-    <t>기본</t>
-  </si>
-  <si>
-    <t>작업 유형</t>
-  </si>
-  <si>
-    <t>대기 모드에서 x{0}%</t>
-  </si>
-  <si>
-    <t>그룹 구역만 사용</t>
-  </si>
-  <si>
-    <t>메카노이드가 그룹에 할당된 구역 내부에서만 작업하도록 제한할 수 있습니다.</t>
-  </si>
-  <si>
-    <t>{0} 설정을 기본값으로 초기화합니다.</t>
-  </si>
-  <si>
-    <t>구역 소유자를 초기화할 수 있습니다.</t>
-  </si>
-  <si>
-    <t>소유자 초기화</t>
-  </si>
-  <si>
-    <t>{0}(이)가 {1}의 소유자로 지정되었습니다.</t>
-  </si>
-  <si>
-    <t>구역 소유자를 지정할 수 있습니다.</t>
-  </si>
-  <si>
-    <t>메카나이터 지정</t>
-  </si>
-  <si>
-    <t>그룹 {0}(을)를 {1}에 할당했습니다.</t>
-  </si>
-  <si>
-    <t>이 구역으로 돌아올 메카노이드 그룹을 지정할 수 있습니다.</t>
-  </si>
-  <si>
-    <t>그룹 지정</t>
-  </si>
-  <si>
-    <t>현재 소유자</t>
-  </si>
-  <si>
-    <t>현재 그룹</t>
-  </si>
-  <si>
-    <t>새로운 작업 유형 사용 가능:</t>
-  </si>
-  <si>
-    <t>요구 연구:</t>
-  </si>
-  <si>
-    <t>{0}(을)를 호위합니다</t>
-  </si>
-  <si>
-    <t>{0}(이)가 더 이상 {1}(을)를 호위하지 않습니다.</t>
-  </si>
-  <si>
-    <t>{0}(이)가 {1}(을)를 호위합니다.</t>
-  </si>
-  <si>
-    <t>{0}(이)가 {1}(을)를 호위함
-메카노이드에게 어떤 정착민을 호위할지 지정할 수 있습니다.
-{0}(은)는 상단이나 정착지 외부의 맵에서 감독관 이외의 다른 사람을 따라갈 수 없습니다.</t>
-  </si>
-  <si>
-    <t>호위 대상 초기화</t>
-  </si>
-  <si>
-    <t>호위 배정</t>
-  </si>
-  <si>
-    <t>셀: {0} | 최소 허용: {1}</t>
-  </si>
-  <si>
-    <t>수집' 유형의 메카노이드는 이 구역에서 유용한 자원을 찾습니다.</t>
-  </si>
-  <si>
-    <t>메카노이드 수집 구역</t>
-  </si>
-  <si>
-    <t>모든 유형의 메카노이드를 이곳에서 대기하도록 합니다.</t>
-  </si>
-  <si>
-    <t>특정 유형의 메카노이드를 이곳에서 대기하도록 합니다.</t>
-  </si>
-  <si>
-    <t>모든 유형 허용</t>
-  </si>
-  <si>
-    <t>매복 유형</t>
-  </si>
-  <si>
-    <t>전투 유형</t>
-  </si>
-  <si>
-    <t>안전 유형</t>
-  </si>
-  <si>
-    <t>노동 유형</t>
-  </si>
-  <si>
-    <t>메카노이드는 이곳으로 돌아와 대기합니다.</t>
-  </si>
-  <si>
-    <t>메카노이드 대기 구역</t>
-  </si>
-  <si>
-    <t>기계 수집</t>
-  </si>
-  <si>
-    <t>메카나이터가 메카노이드에게 고급 작업 명령을 내릴 수 있습니다.</t>
-  </si>
-  <si>
-    <t>기계 연구</t>
+    <t>Keyed+WVC_Label_mechBandwithCostInDormantMode</t>
+  </si>
+  <si>
+    <t>WVC_Label_mechBandwithCostInDormantMode</t>
+  </si>
+  <si>
+    <t>Dormant mode bandwidth cost factor x{0}%</t>
+  </si>
+  <si>
+    <t>메카노이드 휴면 시 대역폭 x{0}%</t>
+  </si>
+  <si>
+    <t>recharge and shutdown</t>
+  </si>
+  <si>
+    <t>MechWorkModeDef+WVC_RechargeAndShutdown.description</t>
+  </si>
+  <si>
+    <t>WVC_RechargeAndShutdown.description</t>
+  </si>
+  <si>
+    <t>Mechanoids, regardless of type, will first go to charge, and then to the shutdown zone.
+&lt;color=#f5ffa2&gt;Type:&lt;/color&gt; Safe
+&lt;color=#f5ffa2&gt;Enemy searching:&lt;/color&gt; No
+&lt;color=#f5ffa2&gt;Shutdown:&lt;/color&gt; Yes
+&lt;color=#f5ffa2&gt;Smart charging:&lt;/color&gt; Yes</t>
+  </si>
+  <si>
+    <t>RoomRoleDef+WVC_MechHangar.label</t>
+  </si>
+  <si>
+    <t>RoomRoleDef</t>
+  </si>
+  <si>
+    <t>WVC_MechHangar.label</t>
+  </si>
+  <si>
+    <t>mechanoid hangar</t>
+  </si>
+  <si>
+    <t>Keyed+WVC_WM_ShutdownGroup</t>
+  </si>
+  <si>
+    <t>WVC_WM_ShutdownGroup</t>
+  </si>
+  <si>
+    <t>shutdown</t>
+  </si>
+  <si>
+    <t>Keyed+WVC_Label_RechargeAndShutdown</t>
+  </si>
+  <si>
+    <t>WVC_Label_RechargeAndShutdown</t>
+  </si>
+  <si>
+    <t>Recharge and shutdown</t>
+  </si>
+  <si>
+    <t>Keyed+WVC_Label_enable_GoToShutdownRoomJob</t>
+  </si>
+  <si>
+    <t>WVC_Label_enable_GoToShutdownRoomJob</t>
+  </si>
+  <si>
+    <t>Enable mechanoid hangar rooms (Beta)</t>
+  </si>
+  <si>
+    <t>Keyed+WVC_ToolTip_enable_GoToShutdownRoomJob</t>
+  </si>
+  <si>
+    <t>WVC_ToolTip_enable_GoToShutdownRoomJob</t>
+  </si>
+  <si>
+    <t>If enabled, all mechanoid chargers will create a new room type "Mechanoid Hangar". Mechanoids will sleep there if there are no alternatives in the form of zones.
+Recommended when playing through gravships (Odyssey DLC), since the zones are reset when the ship flies.
+(Beta) A special beacon is planned that will allow for fine-tuning similar to that with zones.
+Restart required!</t>
+  </si>
+  <si>
+    <t>Keyed+WVC_WM_Label_enableAutoRepairByDefault</t>
+  </si>
+  <si>
+    <t>WVC_WM_Label_enableAutoRepairByDefault</t>
+  </si>
+  <si>
+    <t>Auto-repair on by default</t>
+  </si>
+  <si>
+    <t>Keyed+WVC_WM_ToolTip_enableAutoRepairByDefault</t>
+  </si>
+  <si>
+    <t>WVC_WM_ToolTip_enableAutoRepairByDefault</t>
+  </si>
+  <si>
+    <t>After spawning, automatically switches the mechanoid's auto-repair to true.</t>
+  </si>
+  <si>
+    <t>메카노이드 대기 구역 활성화</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>메카노이드 격납고</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>충전 및 대기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>메카노이드 격납고 방 유형 활성화</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자동 수리 기본 켜기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>메카노이드의 자동 수리를 기본적으로 켭니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>활성화하면 모든 메카노이드 충전기가 새로운 방 유형 "메카노이드 격납고"를 생성합니다. 메카노이드는 구역 형태의 대안이 없으면 그곳에서 잠을 잘 것입니다.\n\n중력부양선(Odyssey DLC)이 비행할 경우 외부 구역이 재설정되기 때문에 권장합니다.\n\n(베타) 구역과 유사한 미세 조정이 가능한 특수 신호기가 계획되어 있습니다.\n\n재시작이 필요합니다!</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>메카노이드는 적이 맵에 없는 한 작업을 수행합니다. 위험이 있을 경우, 안전 지점으로 이동하려고 할 것입니다.\n\n&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 안전, 작업\n&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 사용\n&lt;color=#f5ffa2&gt;정지 지점:&lt;/color&gt; 안전한 지점\n&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 사용</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>메카노이드는 종류에 관계없이 너무 가까이 다가온 적을 공격할 것입니다.\n\n&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 안전\n&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 사용 안함\n&lt;color=#f5ffa2&gt;대기 모드:&lt;/color&gt; 피해를 입음
+\n&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 사용 안함</t>
+  </si>
+  <si>
+    <t>메카노이드는 유형에 관계없이 대역폭 비용에 비례하여 연구 포인트를 생성합니다. 맵에 적이 있거나 피해를 입으면 메카노이드는 안전 지대로 이동합니다.\n\n&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 안전\n&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 사용\n&lt;color=#f5ffa2&gt;대기 모드:&lt;/color&gt; 피해를 입음\n&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 사용 안함</t>
+  </si>
+  <si>
+    <t>메카노이드는 종류에 관계없이 "수집" 구역에서 유용한 자원을 찾습니다. 맵에 적이 있거나 피해를 입으면 메카노이드는 안전 지대로 이동합니다.\n\n&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 안전\n&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 사용\n&lt;color=#f5ffa2&gt;대기 모드:&lt;/color&gt; 피해를 입음\n&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 사용 안함</t>
+  </si>
+  <si>
+    <t>메카노이드는 종류에 관계없이 적을 찾아서 파괴하려고 할 것입니다.\n\n&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 전투\n&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 사용\n&lt;color=#f5ffa2&gt;대기 모드:&lt;/color&gt; 사용 안함\n&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 사용 안함</t>
+  </si>
+  <si>
+    <t>메카노이드는 적이 없으면 대기하고, 적이 나타나면 깨어나서 목표지점으로 향할 것입니다.\n\n&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 전투\n&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 사용\n&lt;color=#f5ffa2&gt;대기 모드:&lt;/color&gt; 사용\n&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 사용 안함</t>
+  </si>
+  <si>
+    <t>메카노이드는 종류에 따라 작업을 수행하며, 적이 나타나면 모든 것을 내려놓고 적을 파괴하러 갈 것입니다. 작업이 없는 경우에는 종료될 것입니다.\n&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 전투\n&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 사용\n&lt;color=#f5ffa2&gt;대기 모드:&lt;/color&gt; 사용\n&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 사용</t>
+  </si>
+  <si>
+    <t>메카노이드는 종료되어 적이 다가올 때까지 기다린 후 공격합니다.\n\n&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 매복\n&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 사용 안함\n&lt;color=#f5ffa2&gt;대기 모드:&lt;/color&gt; 사용\n&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 사용 안함</t>
+  </si>
+  <si>
+    <t>메카노이드는 메카노이드의 종류에 따라 자율적으로 작업을 수행합니다. 만약 메카노이드가 작업을 수행할 수 없거나 모든 작업을 완료했다면 종료됩니다.
+&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 작업
+&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 사용 안함
+&lt;color=#f5ffa2&gt;대기 모드:&lt;/color&gt; 사용
+&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 사용</t>
+  </si>
+  <si>
+    <t>메카노이드는 작업이 없는 경우 감독관과 함께 이동하며 필요한 경우 충전될 것입니다.\n\n&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 전투\n&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 사용 안함\n&lt;color=#f5ffa2&gt;대기 모드:&lt;/color&gt; 사용 안함\n&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 사용 안함</t>
+  </si>
+  <si>
+    <t>메카노이드는 종류에 관계없이 적군이 자신의 작전 구역에 있을 때 감독관과 동행합니다. 그렇지 않으면 평범하게 작업합니다.
+&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 전투
+&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 사용
+&lt;color=#f5ffa2&gt;대기 모드:&lt;/color&gt; 사용
+&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 사용</t>
+  </si>
+  <si>
+    <t>메카노이드는 유형에 관계없이 소집되거나 쓰러질 경우 감독관과 동행합니다.
+&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 전투
+&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 사용 안함
+&lt;color=#f5ffa2&gt;대기 모드:&lt;/color&gt; 사용
+&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 사용</t>
+  </si>
+  <si>
+    <t>메카노이드는 종류에 관계없이 감독관과 함께 이동할 것입니다. 단, 맵에 적이 있는 경우에만 이동합니다. 적이 없을 때는 메카노이드가 종료됩니다.
+&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 전투
+&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 사용
+&lt;color=#f5ffa2&gt;대기 모드:&lt;/color&gt; 사용
+&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 사용</t>
   </si>
   <si>
     <t>메카노이드는 종류에 관계없이 감독관과 함께 이동하며 필요한 경우 충전소로 이동할 것입니다.
 &lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 전투
-&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 아니요
-&lt;color=#f5ffa2&gt;종료 장소:&lt;/color&gt; 아니요
-&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 아니요</t>
-  </si>
-  <si>
-    <t>메카노이드는 종류에 관계없이 감독관과 함께 이동할 것입니다. 단, 맵에 적이 있는 경우에만 이동합니다. 적이 없을 때는 메카노이드가 종료됩니다.
-&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 전투
-&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 예
-&lt;color=#f5ffa2&gt;종료 장소:&lt;/color&gt; 대기 장소
-&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 예</t>
-  </si>
-  <si>
-    <t>메카노이드는 유형에 관계없이 소집되거나 쓰러질 경우 감독관과 동행합니다.
-&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 전투
-&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 아니요
-&lt;color=#f5ffa2&gt;종료 장소:&lt;/color&gt; 예
-&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 예</t>
-  </si>
-  <si>
-    <t>메카노이드는 종류에 관계없이 적군이 자신의 작전 구역에 있을 때 감독관과 동행합니다. 그렇지 않으면 평범하게 작업합니다.
-&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 전투
-&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 예
-&lt;color=#f5ffa2&gt;종료 장소:&lt;/color&gt; 예
-&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 예</t>
-  </si>
-  <si>
-    <t>메카노이드는 작업이 없는 경우 감독관과 함께 이동하며 필요한 경우 충전될 것입니다.
-&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 범용
-&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 아니요
-&lt;color=#f5ffa2&gt;종료 장소:&lt;/color&gt; 아니요
-&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 아니요</t>
-  </si>
-  <si>
-    <t>메카노이드는 적이 맵에 없는 한 작업을 수행합니다. 위험이 있을 경우, 안전 지점으로 이동하려고 할 것입니다.
-&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 작업
-&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 예
-&lt;color=#f5ffa2&gt;정지 지점:&lt;/color&gt; 안전한 지점
-&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 예</t>
-  </si>
-  <si>
-    <t>메카노이드는 메카노이드의 종류에 따라 자율적으로 작업을 수행합니다. 만약 메카노이드가 작업을 수행할 수 없거나 모든 작업을 완료했다면 종료됩니다.
-&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 작업
-&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 아니요
-&lt;color=#f5ffa2&gt;종료 장소:&lt;/color&gt; 작업자 지점
-&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 예</t>
-  </si>
-  <si>
-    <t>메카노이드는 종료되어 적이 다가올 때까지 기다린 후 공격합니다.
-&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 전투
-&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 아니요
-&lt;color=#f5ffa2&gt;종료 장소:&lt;/color&gt; 매복 지점
-&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 아니요</t>
-  </si>
-  <si>
-    <t>메카노이드는 종류에 따라 작업을 수행하며, 적이 나타나면 모든 것을 내려놓고 적을 파괴하러 갈 것입니다. 작업이 없는 경우에는 종료될 것입니다.
-&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 범용
-&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 예
-&lt;color=#f5ffa2&gt;종료 장소:&lt;/color&gt; 대기 장소
-&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 예</t>
-  </si>
-  <si>
-    <t>메카노이드는 적이 없으면 대기하고, 적이 나타나면 깨어나서 목표지점으로 향할 것입니다.
-&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 전투
-&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 예
-&lt;color=#f5ffa2&gt;종료 장소:&lt;/color&gt; 대기 장소
-&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 아니요</t>
-  </si>
-  <si>
-    <t>메카노이드는 종류에 관계없이 적을 찾아서 파괴하려고 할 것입니다.
-&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 전투
-&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 예
-&lt;color=#f5ffa2&gt;종료 장소:&lt;/color&gt; 아니요
-&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 예</t>
-  </si>
-  <si>
-    <t>메카노이드는 종류에 관계없이 "수집" 구역에서 유용한 자원을 찾습니다.
-맵에 적이 있거나 피해를 입으면 메카노이드는 안전 지대로 이동합니다.
-&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 안전
-&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 아니요
-&lt;color=#f5ffa2&gt;종료 장소:&lt;/color&gt; 피해를 입음
-&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 예</t>
-  </si>
-  <si>
-    <t>메카노이드는 유형에 관계없이 대역폭 비용에 비례하여 연구 포인트를 생성합니다. 연구 속도와 효율은 연구에 참여하는 메카노이드의 수에 따라 직접적으로 달라집니다.
-맵에 적이 있거나 피해를 입으면 메카노이드는 안전 지대로 이동합니다.
-&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 안전
-&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 아니요
-&lt;color=#f5ffa2&gt;종료 장소:&lt;/color&gt; 피해를 입음
-&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 예</t>
-  </si>
-  <si>
-    <t>메카노이드는 종류에 관계없이 너무 가까이 다가온 적을 공격할 것입니다.
-&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 없음
-&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 아니요
-&lt;color=#f5ffa2&gt;종료 장소:&lt;/color&gt; 아니요
-&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 아니요</t>
-  </si>
-  <si>
-    <t>이 모드는 알아두어야 할 몇 가지 독특한 동작을 추가합니다.
--
-지도에서 적을 확인합니다. 적이 접근 가능하고 메카노이드가 작동하는 영역에 없다면 메카노이드는 정상적으로 작동을 계속합니다.
-무엇을 의미하는가:
-"안전한 경우 작업" 모드를 활성화하고 작업 영역을 제한하면, 메카노이드는 적이 메카노이드의 작업 영역에 들어올 때까지 침입을 무시합니다.
-"소탕" 모드를 활성화하고 메카노이드를 작지만 개방된 영역에 고정시킨 경우, 메카노이드는 적을 추적하지 않고 메카노이드의 시야에 있는 적과 싸우려고 할 것입니다. 지나치게 스마트한 적 AI 모드를 깔았다면 메카노이드를 카이팅할 수도 있습니다.
--
-자동 충전 - 일부 모드에서 메카노이드는 최대 충전량에 가깝도록 유지하려고 합니다. 이는 다음 공식에 따라 계산됩니다 (최대 충전 수준 - 5). 즉, 충전을 100%로 설정하면 메카노이드는 95%까지 충전됩니다. 그러나 기본 충전과 달리, 필요한 경우 메카노이드는 충전을 중단합니다.
--
-대기 모드 - 일부 작업 모드에서는 아무것도 하지 않을 때 최적화를 위해 메카노이드를 비활성화합니다. 작업 모드에서는 재사용 대기시간이 전투 모드보다 훨씬 길어집니다.
--
-메카노이드 대기 구역 - 모든 업무를 마치고 잠들려고 하는 메카노이드는 접근 가능한 구역에 있는 경우 가장 가까운 구역으로 이동합니다.
--
-스마트 호위 - 메카노이드에 호위 대상을 지정할 수 있습니다. 메카노이드가 다른 폰을 보호하고 동행합니다. 이 기능은 정착지에서만 작동합니다.</t>
-  </si>
-  <si>
-    <t>더 많은 메카노이드 작업 모드 - 동작들</t>
-  </si>
-  <si>
-    <t>{0}(이)가 연구되지 않아 사용할 수 없습니다. {1} 유형으로 변경됩니다.</t>
+&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 사용 안함
+&lt;color=#f5ffa2&gt;대기 모드:&lt;/color&gt; 사용 안함
+&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 사용 안함</t>
+  </si>
+  <si>
+    <t>'수집' 유형의 메카노이드는 이 구역에서 유용한 자원을 찾습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>비활성화하기 전에 모든 메카노이드 모드를 바닐라로 전환하세요. 설정을 적용하려면 재시작해야 합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>메카노이드는 종류에 관계없이 먼저 충전한 다음 대기 구역으로 이동합니다.\n\n&lt;color=#f5ffa2&gt;유형:&lt;/color&gt; 안전\n&lt;color=#f5ffa2&gt;적 수색:&lt;/color&gt; 사용 안함\n&lt;color=#f5ffa2&gt;대기 모드:&lt;/color&gt; 사용\n&lt;color=#f5ffa2&gt;스마트 충전:&lt;/color&gt; 사용</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1592,7 +1871,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1611,13 +1890,41 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF87CEEB"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1632,9 +1939,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1936,11 +2248,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F119"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="C109" workbookViewId="0">
+      <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1949,9 +2261,10 @@
     <col min="2" max="2" width="20.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="43.08984375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="5" max="5" width="49.26953125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="43.08984375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -1967,10 +2280,10 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1984,10 +2297,7 @@
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2001,1987 +2311,2129 @@
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>459</v>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>458</v>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>396</v>
+        <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>457</v>
+        <v>28</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>386</v>
+        <v>31</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>456</v>
+        <v>35</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>385</v>
+        <v>38</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>455</v>
+      <c r="F11" s="2" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>399</v>
+        <v>45</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>454</v>
+      <c r="F13" s="2" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>398</v>
+        <v>52</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>453</v>
+        <v>56</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>397</v>
+        <v>59</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>452</v>
+        <v>63</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>395</v>
+        <v>66</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>451</v>
+        <v>70</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>394</v>
+        <v>73</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>450</v>
+        <v>77</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>393</v>
+        <v>80</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>449</v>
+        <v>84</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>391</v>
+        <v>87</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>448</v>
+        <v>91</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>388</v>
+        <v>94</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>447</v>
+        <v>98</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>387</v>
+        <v>101</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>446</v>
+        <v>105</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>390</v>
+        <v>108</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>445</v>
+        <v>112</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>392</v>
+        <v>115</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>444</v>
+        <v>119</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>442</v>
+        <v>123</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>443</v>
+        <v>127</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>442</v>
+        <v>130</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>441</v>
+        <v>132</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>440</v>
+        <v>137</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>439</v>
+        <v>141</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>438</v>
+        <v>145</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>437</v>
+        <v>149</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>130</v>
+        <v>152</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>436</v>
+        <v>153</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>435</v>
+        <v>157</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>434</v>
+        <v>161</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>433</v>
+        <v>165</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>432</v>
+        <v>169</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>147</v>
+        <v>173</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>150</v>
+        <v>176</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>431</v>
+        <v>179</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>430</v>
+        <v>183</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>157</v>
+        <v>185</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>429</v>
+        <v>186</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>160</v>
+        <v>189</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>428</v>
+        <v>190</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>427</v>
+        <v>194</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>166</v>
+        <v>197</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>426</v>
+        <v>198</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>169</v>
+        <v>201</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>425</v>
+        <v>202</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>172</v>
+        <v>205</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>424</v>
+        <v>206</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>423</v>
+        <v>210</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>178</v>
+        <v>213</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>460</v>
+        <v>214</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
-        <v>181</v>
+        <v>216</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>422</v>
+        <v>218</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>184</v>
+        <v>221</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>421</v>
+        <v>222</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
-        <v>187</v>
+        <v>225</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>189</v>
+        <v>226</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>190</v>
+        <v>228</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>420</v>
+        <v>229</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>193</v>
+        <v>232</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>419</v>
+        <v>233</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
-        <v>196</v>
+        <v>236</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>418</v>
+        <v>237</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>199</v>
+        <v>240</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>417</v>
+        <v>241</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>202</v>
+        <v>244</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>416</v>
+        <v>245</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>205</v>
+        <v>248</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>415</v>
+        <v>249</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>208</v>
+        <v>252</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>414</v>
+        <v>253</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>211</v>
+        <v>256</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>413</v>
+        <v>257</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>214</v>
+        <v>260</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>412</v>
+        <v>261</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>217</v>
+        <v>264</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>411</v>
+        <v>265</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>220</v>
+        <v>268</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>410</v>
+        <v>269</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>223</v>
+        <v>272</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>408</v>
+        <v>273</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
-        <v>226</v>
+        <v>276</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>409</v>
+        <v>277</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
-        <v>229</v>
+        <v>280</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>408</v>
+        <v>281</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
-        <v>232</v>
+        <v>283</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>407</v>
+        <v>284</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
-        <v>235</v>
+        <v>287</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>406</v>
+        <v>288</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
-        <v>238</v>
+        <v>291</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>405</v>
+        <v>292</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
-        <v>241</v>
+        <v>295</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>404</v>
+        <v>296</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
-        <v>244</v>
+        <v>299</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>403</v>
+        <v>300</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
-        <v>247</v>
+        <v>303</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>402</v>
+        <v>304</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
-        <v>250</v>
+        <v>307</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>401</v>
+        <v>308</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
-        <v>253</v>
+        <v>311</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>400</v>
+        <v>312</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
-        <v>256</v>
+        <v>315</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>399</v>
+        <v>316</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
-        <v>259</v>
+        <v>318</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>398</v>
+        <v>319</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
-        <v>262</v>
+        <v>321</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>397</v>
+        <v>322</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
-        <v>265</v>
+        <v>324</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>396</v>
+        <v>325</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
-        <v>268</v>
+        <v>327</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>395</v>
+        <v>328</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
-        <v>271</v>
+        <v>330</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>394</v>
+        <v>331</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" s="1" t="s">
-        <v>274</v>
+        <v>333</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>393</v>
+        <v>334</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" s="1" t="s">
-        <v>277</v>
+        <v>336</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>392</v>
+        <v>337</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
-        <v>280</v>
+        <v>339</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>391</v>
+        <v>340</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
-        <v>283</v>
+        <v>342</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>390</v>
+        <v>343</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
-        <v>286</v>
+        <v>345</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>389</v>
+        <v>346</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" s="1" t="s">
-        <v>289</v>
+        <v>348</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>388</v>
+        <v>349</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" s="1" t="s">
-        <v>292</v>
+        <v>351</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>387</v>
+        <v>352</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" s="1" t="s">
-        <v>295</v>
+        <v>354</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>386</v>
+        <v>355</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" s="1" t="s">
-        <v>298</v>
+        <v>357</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>385</v>
+        <v>358</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" s="1" t="s">
-        <v>301</v>
+        <v>360</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>384</v>
+        <v>361</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" s="1" t="s">
-        <v>304</v>
+        <v>364</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>383</v>
+        <v>365</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" s="1" t="s">
-        <v>307</v>
+        <v>368</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E101" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>382</v>
+        <v>369</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102" s="1" t="s">
-        <v>310</v>
+        <v>372</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>381</v>
+        <v>373</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103" s="1" t="s">
-        <v>313</v>
+        <v>376</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104" s="1" t="s">
-        <v>316</v>
+        <v>380</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>379</v>
+        <v>381</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105" s="1" t="s">
-        <v>319</v>
+        <v>384</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="F105" s="1" t="s">
-        <v>378</v>
+        <v>385</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106" s="1" t="s">
-        <v>322</v>
+        <v>388</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>377</v>
+        <v>389</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A107" s="1" t="s">
-        <v>325</v>
+        <v>391</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>376</v>
+        <v>392</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A108" s="1" t="s">
-        <v>328</v>
+        <v>395</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>375</v>
+        <v>396</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A109" s="1" t="s">
-        <v>331</v>
+        <v>399</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>374</v>
+        <v>400</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A110" s="1" t="s">
-        <v>334</v>
+        <v>403</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>373</v>
+        <v>404</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A111" s="1" t="s">
-        <v>337</v>
+        <v>407</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>372</v>
+        <v>408</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A112" s="1" t="s">
-        <v>340</v>
+        <v>411</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>371</v>
+        <v>412</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A113" s="1" t="s">
-        <v>343</v>
+        <v>415</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="E113" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>370</v>
+        <v>416</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A114" s="1" t="s">
-        <v>346</v>
+        <v>419</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="E114" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>369</v>
+        <v>420</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A115" s="1" t="s">
-        <v>349</v>
+        <v>423</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>368</v>
+        <v>424</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A116" s="1" t="s">
-        <v>352</v>
+        <v>427</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="E116" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>367</v>
+        <v>428</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A117" s="1" t="s">
-        <v>355</v>
+        <v>431</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>366</v>
+        <v>432</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A118" s="1" t="s">
-        <v>358</v>
+        <v>435</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>365</v>
+        <v>436</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A119" s="1" t="s">
-        <v>361</v>
+        <v>439</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>364</v>
+        <v>440</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A121" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E121" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A122" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A123" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A124" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A125" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A126" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A127" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A128" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A129" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>475</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>